<commit_message>
Generated N_xi, T_xi vs FWHM
</commit_message>
<xml_diff>
--- a/paper_analysis/Results/Results (PW=False, BW=50Hz, Static Flattop)/N_xi Fitted Parameters (Static Flattop, PW=False, BW=50Hz).xlsx
+++ b/paper_analysis/Results/Results (PW=False, BW=50Hz, Static Flattop)/N_xi Fitted Parameters (Static Flattop, PW=False, BW=50Hz).xlsx
@@ -1283,31 +1283,31 @@
         <v>2804.69970703125</v>
       </c>
       <c r="E19" t="n">
-        <v>78.72239662265706</v>
+        <v>113.9591263556091</v>
       </c>
       <c r="F19" t="n">
-        <v>3.950777401015761</v>
+        <v>4.490614335708175</v>
       </c>
       <c r="G19" t="n">
-        <v>0.02806803039387915</v>
+        <v>0.04063148937831701</v>
       </c>
       <c r="H19" t="n">
-        <v>0.001408627594288026</v>
+        <v>0.0016011034352271</v>
       </c>
       <c r="I19" t="n">
-        <v>0.9342546231075746</v>
+        <v>0.779465647665269</v>
       </c>
       <c r="J19" t="n">
-        <v>0.03272267620462239</v>
+        <v>0.02275662711473331</v>
       </c>
       <c r="K19" t="n">
-        <v>0.002807780409620144</v>
+        <v>0.003001105705378799</v>
       </c>
       <c r="L19" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.1017687074829932</v>
       </c>
       <c r="M19" t="n">
-        <v>139.9169921875</v>
+        <v>285.4306640625</v>
       </c>
     </row>
     <row r="20">
@@ -1328,31 +1328,31 @@
         <v>2944.66552734375</v>
       </c>
       <c r="E20" t="n">
-        <v>151.3031536114009</v>
+        <v>206.131525272019</v>
       </c>
       <c r="F20" t="n">
-        <v>6.36812233398685</v>
+        <v>2.992513499515958</v>
       </c>
       <c r="G20" t="n">
-        <v>0.0513821186842516</v>
+        <v>0.07000167705225285</v>
       </c>
       <c r="H20" t="n">
-        <v>0.002162596150514672</v>
+        <v>0.001016249034645157</v>
       </c>
       <c r="I20" t="n">
-        <v>0.9121406350637296</v>
+        <v>0.814203945606629</v>
       </c>
       <c r="J20" t="n">
-        <v>0.01831182889403164</v>
+        <v>0.008360030886865192</v>
       </c>
       <c r="K20" t="n">
-        <v>0.001266257768043677</v>
+        <v>0.0007921288007696902</v>
       </c>
       <c r="L20" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.164625850340136</v>
       </c>
       <c r="M20" t="n">
-        <v>146.8994140625</v>
+        <v>484.76806640625</v>
       </c>
     </row>
     <row r="21">
@@ -1373,31 +1373,31 @@
         <v>3865.2099609375</v>
       </c>
       <c r="E21" t="n">
-        <v>257.5285352144602</v>
+        <v>344.7310563671853</v>
       </c>
       <c r="F21" t="n">
-        <v>10.41880586101659</v>
+        <v>3.212280051220951</v>
       </c>
       <c r="G21" t="n">
-        <v>0.06662730817137735</v>
+        <v>0.08918818378590004</v>
       </c>
       <c r="H21" t="n">
-        <v>0.00269553425721006</v>
+        <v>0.000831075176687638</v>
       </c>
       <c r="I21" t="n">
-        <v>0.9003194522879659</v>
+        <v>0.8240408610291559</v>
       </c>
       <c r="J21" t="n">
-        <v>0.01437699973941896</v>
+        <v>0.005257218580075067</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0008017202448917241</v>
+        <v>0.0003960369318489034</v>
       </c>
       <c r="L21" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.1905668934240363</v>
       </c>
       <c r="M21" t="n">
-        <v>192.822265625</v>
+        <v>736.5810546875</v>
       </c>
     </row>
     <row r="22">
@@ -1418,31 +1418,31 @@
         <v>2341.73583984375</v>
       </c>
       <c r="E22" t="n">
-        <v>1238.987999586158</v>
+        <v>834.305292338149</v>
       </c>
       <c r="F22" t="n">
-        <v>27.14368837184672</v>
+        <v>3.085547371749579</v>
       </c>
       <c r="G22" t="n">
-        <v>0.5290895661693541</v>
+        <v>0.3562764331239928</v>
       </c>
       <c r="H22" t="n">
-        <v>0.01159126828483688</v>
+        <v>0.001317632552421224</v>
       </c>
       <c r="I22" t="n">
-        <v>0.9985559661637051</v>
+        <v>1.133083655028301</v>
       </c>
       <c r="J22" t="n">
-        <v>0.001157693446857856</v>
+        <v>0.00318565913538339</v>
       </c>
       <c r="K22" t="n">
-        <v>1.455369872586139e-05</v>
+        <v>0.0003926930286779309</v>
       </c>
       <c r="L22" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.791201814058957</v>
       </c>
       <c r="M22" t="n">
-        <v>116.8212890625</v>
+        <v>1852.78564453125</v>
       </c>
     </row>
     <row r="23">
@@ -1463,31 +1463,31 @@
         <v>4048.2421875</v>
       </c>
       <c r="E23" t="n">
-        <v>1119.647986584904</v>
+        <v>915.1772653853163</v>
       </c>
       <c r="F23" t="n">
-        <v>102.1722308957542</v>
+        <v>4.711981334085687</v>
       </c>
       <c r="G23" t="n">
-        <v>0.2765763347959043</v>
+        <v>0.2260678148681825</v>
       </c>
       <c r="H23" t="n">
-        <v>0.02523866561423562</v>
+        <v>0.001163957371086926</v>
       </c>
       <c r="I23" t="n">
-        <v>0.8713341333412855</v>
+        <v>0.9355280090025678</v>
       </c>
       <c r="J23" t="n">
-        <v>0.008827989326729105</v>
+        <v>0.003187951297108425</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0003364991741366163</v>
+        <v>0.0004252168081894256</v>
       </c>
       <c r="L23" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.4779138321995465</v>
       </c>
       <c r="M23" t="n">
-        <v>201.953125</v>
+        <v>1934.7109375</v>
       </c>
     </row>
     <row r="24">
@@ -1508,31 +1508,31 @@
         <v>5840.88134765625</v>
       </c>
       <c r="E24" t="n">
-        <v>451.5425013612262</v>
+        <v>561.3404051986048</v>
       </c>
       <c r="F24" t="n">
-        <v>18.67375986188917</v>
+        <v>3.692902305989144</v>
       </c>
       <c r="G24" t="n">
-        <v>0.07730725458794246</v>
+        <v>0.09610542857951598</v>
       </c>
       <c r="H24" t="n">
-        <v>0.003197079130768907</v>
+        <v>0.0006322508686931267</v>
       </c>
       <c r="I24" t="n">
-        <v>0.8998060709635739</v>
+        <v>0.8471350160927504</v>
       </c>
       <c r="J24" t="n">
-        <v>0.01317624744019336</v>
+        <v>0.003825152408858302</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0006434922576667309</v>
+        <v>0.0002201594302102151</v>
       </c>
       <c r="L24" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.2035374149659864</v>
       </c>
       <c r="M24" t="n">
-        <v>291.3818359375</v>
+        <v>1188.837890625</v>
       </c>
     </row>
     <row r="25">
@@ -1553,31 +1553,31 @@
         <v>8311.81640625</v>
       </c>
       <c r="E25" t="n">
-        <v>1753.631264694655</v>
+        <v>1499.80490094161</v>
       </c>
       <c r="F25" t="n">
-        <v>54.99792277194764</v>
+        <v>6.673417182006846</v>
       </c>
       <c r="G25" t="n">
-        <v>0.2109805100334058</v>
+        <v>0.180442496277209</v>
       </c>
       <c r="H25" t="n">
-        <v>0.006616835608952145</v>
+        <v>0.0008028831311756148</v>
       </c>
       <c r="I25" t="n">
-        <v>0.9362753106151652</v>
+        <v>0.9913508991671014</v>
       </c>
       <c r="J25" t="n">
-        <v>0.004470411392156343</v>
+        <v>0.003151769258650574</v>
       </c>
       <c r="K25" t="n">
-        <v>5.24716086802395e-05</v>
+        <v>0.000302896325251435</v>
       </c>
       <c r="L25" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.4489795918367347</v>
       </c>
       <c r="M25" t="n">
-        <v>414.6484375</v>
+        <v>3731.8359375</v>
       </c>
     </row>
     <row r="26">
@@ -1598,31 +1598,31 @@
         <v>732.12890625</v>
       </c>
       <c r="E26" t="n">
-        <v>47.44190869994463</v>
+        <v>466.0924839211502</v>
       </c>
       <c r="F26" t="n">
-        <v>5.251936765771554</v>
+        <v>3.800331024972224</v>
       </c>
       <c r="G26" t="n">
-        <v>0.06479993932071935</v>
+        <v>0.6366262552157633</v>
       </c>
       <c r="H26" t="n">
-        <v>0.007173513736361306</v>
+        <v>0.005190794944073039</v>
       </c>
       <c r="I26" t="n">
-        <v>0.7741652017163103</v>
+        <v>0.534627006228291</v>
       </c>
       <c r="J26" t="n">
-        <v>0.03328039039741743</v>
+        <v>0.002447408573123219</v>
       </c>
       <c r="K26" t="n">
-        <v>0.005418505073083322</v>
+        <v>0.0007330848403451344</v>
       </c>
       <c r="L26" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.9777777777777777</v>
       </c>
       <c r="M26" t="n">
-        <v>36.5234375</v>
+        <v>715.859375</v>
       </c>
     </row>
     <row r="27">
@@ -1643,31 +1643,31 @@
         <v>985.14404296875</v>
       </c>
       <c r="E27" t="n">
-        <v>475.0303614574664</v>
+        <v>695.310769333164</v>
       </c>
       <c r="F27" t="n">
-        <v>35.92939143691685</v>
+        <v>3.619511561955766</v>
       </c>
       <c r="G27" t="n">
-        <v>0.4821938120094129</v>
+        <v>0.7057960450512719</v>
       </c>
       <c r="H27" t="n">
-        <v>0.03647120610773117</v>
+        <v>0.003674093740696335</v>
       </c>
       <c r="I27" t="n">
-        <v>0.4629818047714407</v>
+        <v>0.49737590322112</v>
       </c>
       <c r="J27" t="n">
-        <v>0.003263965643581124</v>
+        <v>0.001958661161228394</v>
       </c>
       <c r="K27" t="n">
-        <v>2.033737714293203e-07</v>
+        <v>0.0002280282135326375</v>
       </c>
       <c r="L27" t="n">
-        <v>0.04988662131519275</v>
+        <v>1.368888888888889</v>
       </c>
       <c r="M27" t="n">
-        <v>49.1455078125</v>
+        <v>1348.552734375</v>
       </c>
     </row>
     <row r="28">
@@ -1688,31 +1688,31 @@
         <v>1636.5234375</v>
       </c>
       <c r="E28" t="n">
-        <v>41.0027271787391</v>
+        <v>74.70407483815406</v>
       </c>
       <c r="F28" t="n">
-        <v>2.678305867054714</v>
+        <v>4.120631514757928</v>
       </c>
       <c r="G28" t="n">
-        <v>0.02505477540937393</v>
+        <v>0.04564803236321145</v>
       </c>
       <c r="H28" t="n">
-        <v>0.001636582651786626</v>
+        <v>0.002517917813051748</v>
       </c>
       <c r="I28" t="n">
-        <v>0.8990441772837184</v>
+        <v>0.6638039647657984</v>
       </c>
       <c r="J28" t="n">
-        <v>0.04356361394164251</v>
+        <v>0.02649283590623222</v>
       </c>
       <c r="K28" t="n">
-        <v>0.004371360048666435</v>
+        <v>0.00474139839117379</v>
       </c>
       <c r="L28" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.1087528344671202</v>
       </c>
       <c r="M28" t="n">
-        <v>81.640625</v>
+        <v>177.9765625</v>
       </c>
     </row>
     <row r="29">
@@ -1733,31 +1733,31 @@
         <v>2228.6865234375</v>
       </c>
       <c r="E29" t="n">
-        <v>428.0801964636898</v>
+        <v>664.3693275237879</v>
       </c>
       <c r="F29" t="n">
-        <v>52.28455683072881</v>
+        <v>2.762103885001939</v>
       </c>
       <c r="G29" t="n">
-        <v>0.1920773477839422</v>
+        <v>0.2980990464729299</v>
       </c>
       <c r="H29" t="n">
-        <v>0.02345980750585135</v>
+        <v>0.001239341583464014</v>
       </c>
       <c r="I29" t="n">
-        <v>0.8141752176229635</v>
+        <v>0.8021279571210939</v>
       </c>
       <c r="J29" t="n">
-        <v>0.01526521432146054</v>
+        <v>0.002174705061483885</v>
       </c>
       <c r="K29" t="n">
-        <v>0.001164300140417746</v>
+        <v>0.0002823386961817188</v>
       </c>
       <c r="L29" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.6345578231292517</v>
       </c>
       <c r="M29" t="n">
-        <v>111.181640625</v>
+        <v>1414.23046875</v>
       </c>
     </row>
     <row r="30">
@@ -1778,31 +1778,31 @@
         <v>904.39453125</v>
       </c>
       <c r="E30" t="n">
-        <v>439.5041774290074</v>
+        <v>341.5342028676439</v>
       </c>
       <c r="F30" t="n">
-        <v>26.72352902072796</v>
+        <v>1.082528742161299</v>
       </c>
       <c r="G30" t="n">
-        <v>0.4859650984637766</v>
+        <v>0.3776385095955808</v>
       </c>
       <c r="H30" t="n">
-        <v>0.02954853009094637</v>
+        <v>0.001196965157081492</v>
       </c>
       <c r="I30" t="n">
-        <v>0.5090461396223113</v>
+        <v>0.5626423789350109</v>
       </c>
       <c r="J30" t="n">
-        <v>0.002708657780581733</v>
+        <v>0.001445256411606954</v>
       </c>
       <c r="K30" t="n">
-        <v>6.613415558112097e-07</v>
+        <v>6.163483302606143e-05</v>
       </c>
       <c r="L30" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.8241269841269842</v>
       </c>
       <c r="M30" t="n">
-        <v>45.1171875</v>
+        <v>745.3359375</v>
       </c>
     </row>
     <row r="31">
@@ -1823,31 +1823,31 @@
         <v>1518.0908203125</v>
       </c>
       <c r="E31" t="n">
-        <v>363.8420496474109</v>
+        <v>721.8522452495334</v>
       </c>
       <c r="F31" t="n">
-        <v>38.67020613172432</v>
+        <v>1.407005759211592</v>
       </c>
       <c r="G31" t="n">
-        <v>0.2396708054479334</v>
+        <v>0.4755000396491033</v>
       </c>
       <c r="H31" t="n">
-        <v>0.02547292007454734</v>
+        <v>0.0009268258133080334</v>
       </c>
       <c r="I31" t="n">
-        <v>0.8441501564577933</v>
+        <v>0.7922880551757865</v>
       </c>
       <c r="J31" t="n">
-        <v>0.01129200387243904</v>
+        <v>0.0009660258536923005</v>
       </c>
       <c r="K31" t="n">
-        <v>0.0005976880305243168</v>
+        <v>8.879827266136255e-05</v>
       </c>
       <c r="L31" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.9149206349206349</v>
       </c>
       <c r="M31" t="n">
-        <v>75.732421875</v>
+        <v>1388.9326171875</v>
       </c>
     </row>
     <row r="32">
@@ -1868,31 +1868,31 @@
         <v>2040.27099609375</v>
       </c>
       <c r="E32" t="n">
-        <v>372.3325032791528</v>
+        <v>404.0044063224344</v>
       </c>
       <c r="F32" t="n">
-        <v>12.1141797943163</v>
+        <v>0.9558012446096318</v>
       </c>
       <c r="G32" t="n">
-        <v>0.1824916905607201</v>
+        <v>0.1980150710841505</v>
       </c>
       <c r="H32" t="n">
-        <v>0.005937534679221435</v>
+        <v>0.0004684677900335711</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9202134009377445</v>
+        <v>0.9222648903352354</v>
       </c>
       <c r="J32" t="n">
-        <v>0.005101278938237269</v>
+        <v>0.001469159433953898</v>
       </c>
       <c r="K32" t="n">
-        <v>8.297920349893283e-05</v>
+        <v>7.365613627235043e-05</v>
       </c>
       <c r="L32" t="n">
-        <v>0.04988662131519275</v>
+        <v>0.4200453514739229</v>
       </c>
       <c r="M32" t="n">
-        <v>101.7822265625</v>
+        <v>857.00634765625</v>
       </c>
     </row>
     <row r="33">

</xml_diff>